<commit_message>
add helpers and second exam and check internet
</commit_message>
<xml_diff>
--- a/public/file/ExportFormQuestions.xlsx
+++ b/public/file/ExportFormQuestions.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emad\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emad\PhpstormProjects\managment_exams\public\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CA9AB8-CA65-4082-B110-3C96EF2F7300}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05BC454C-578F-4D5D-BE42-BCF77F509D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
+    <sheet name="sourse choose" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>title</t>
   </si>
@@ -51,19 +52,43 @@
     <t>answer</t>
   </si>
   <si>
-    <t>aaa</t>
-  </si>
-  <si>
     <t>صح/خطأ</t>
   </si>
   <si>
     <t>صعب</t>
   </si>
   <si>
-    <t>aaaa</t>
-  </si>
-  <si>
-    <t>aaaaa</t>
+    <t>ما هي عاصمة فلسطين؟</t>
+  </si>
+  <si>
+    <t>اختر</t>
+  </si>
+  <si>
+    <t>سهل</t>
+  </si>
+  <si>
+    <t>متوسط</t>
+  </si>
+  <si>
+    <t>القدس</t>
+  </si>
+  <si>
+    <t>غزة</t>
+  </si>
+  <si>
+    <t>رفح</t>
+  </si>
+  <si>
+    <t>خانيونس</t>
+  </si>
+  <si>
+    <t>صح</t>
+  </si>
+  <si>
+    <t>خطأ</t>
+  </si>
+  <si>
+    <t>لغة البرمجة المسخدمة في برمحة المواقع هي PHP ؟</t>
   </si>
 </sst>
 </file>
@@ -426,18 +451,19 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.28515625" customWidth="1"/>
-    <col min="2" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="39.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -468,54 +494,135 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="9">
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="B1 B3:B1048576" xr:uid="{228B6D60-AEF2-40F5-91D9-1A236980E1D6}">
-      <formula1>"صح/خطأ,أختر"</formula1>
-    </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="متسوى السؤال" prompt="صعب_x000a_متوسط_x000a_سهل" sqref="C1:C1048576" xr:uid="{A6C8B5E8-9510-40DF-B8D2-8255DFE42F04}">
-      <formula1>$C:$C</formula1>
-    </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="نوع السؤال" prompt="صح/خطأ_x000a_اختر" sqref="B2" xr:uid="{BA3624DB-8F91-4A54-8D8C-91D5D3234214}">
-      <formula1>$B:$B</formula1>
-    </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="اختر الخيار الصحيح" prompt="A(صح)_x000a_B(خطأ)_x000a_C_x000a_D" sqref="H1:H1048576" xr:uid="{C3516E0D-FEF3-41BA-A5C3-C45B9EE95350}">
-      <formula1>$H:$H</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="نص السؤال" prompt="يرجى كتابة النص السؤال هنا" sqref="A2" xr:uid="{319A263C-F1CB-4901-9971-51379A6BF5BD}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="الاختيار الاول" prompt="يرجى ادخال الخيار الاول (اجباري)_x000a_يرجى ادخال النص (صح) اذا اخترت نوع السؤال (صح/خطأ)" sqref="D2" xr:uid="{86F33936-87BD-41F2-A861-FE1792501A1F}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="الخيار الثاني " prompt="يرجى ادخال الخيار الثاني (اجباري)_x000a_يرجى ادخال النص (خطأ) اذا اخترت نوع السؤال (صح/خطأ)" sqref="E2" xr:uid="{487D7DAA-AF9A-4EEC-9B91-1ED15C8D7C82}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="الخيار الثالث" prompt="يرجى ادخال الخيار الثالث (اختياري)" sqref="F2" xr:uid="{23C65F67-F181-4A13-B127-8E84AB902834}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="الخيار الرابع" prompt="يرجى ادخال الخيار الرابع (اختياري)" sqref="G2" xr:uid="{86DB4952-79D4-4037-80A1-CAB66DC8C61A}"/>
+  <dataValidations count="5">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="نص السؤال" prompt="يرجى كتابة النص السؤال هنا" sqref="A2:A3" xr:uid="{319A263C-F1CB-4901-9971-51379A6BF5BD}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="الاختيار الاول" prompt="يرجى ادخال الخيار الاول (اجباري)_x000a_يرجى ادخال النص (صح) اذا اخترت نوع السؤال (صح/خطأ)" sqref="D2:D3" xr:uid="{86F33936-87BD-41F2-A861-FE1792501A1F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="الخيار الثاني " prompt="يرجى ادخال الخيار الثاني (اجباري)_x000a_يرجى ادخال النص (خطأ) اذا اخترت نوع السؤال (صح/خطأ)" sqref="E2:E3" xr:uid="{487D7DAA-AF9A-4EEC-9B91-1ED15C8D7C82}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="الخيار الثالث" prompt="يرجى ادخال الخيار الثالث (اختياري)" sqref="F2:F3" xr:uid="{23C65F67-F181-4A13-B127-8E84AB902834}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="الخيار الرابع" prompt="يرجى ادخال الخيار الرابع (اختياري)" sqref="G2:G3" xr:uid="{86DB4952-79D4-4037-80A1-CAB66DC8C61A}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="متسوى السؤال" prompt="صعب_x000a_متوسط_x000a_سهل" xr:uid="{A6C8B5E8-9510-40DF-B8D2-8255DFE42F04}">
+          <x14:formula1>
+            <xm:f>'sourse choose'!$F$1:$F$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>C1:C1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="اختر الخيار الصحيح" prompt="A(صح)_x000a_B(خطأ)_x000a_C_x000a_D" xr:uid="{C3516E0D-FEF3-41BA-A5C3-C45B9EE95350}">
+          <x14:formula1>
+            <xm:f>'sourse choose'!$D$1:$D$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>H1:H1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="يرجى ادخال نوع السؤال" prompt="صح/خطأ_x000a_اختر" xr:uid="{8553585F-05C4-4B75-ABF4-F71F7CF400C2}">
+          <x14:formula1>
+            <xm:f>'sourse choose'!$A$1:$A$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:B1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5668BDAB-9037-4335-998D-4F2775DDE1A6}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>